<commit_message>
Add chat routes with proper authentication and Vercel configuration
- Add chatRoutes.js with secure authentication middleware
- Add vercel.json for deployment configuration
- Fix Vercel security scanner issues
</commit_message>
<xml_diff>
--- a/backend/expense_details.xlsx
+++ b/backend/expense_details.xlsx
@@ -416,24 +416,24 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Game Controller</v>
+        <v xml:space="preserve">Rent </v>
       </c>
       <c r="B2">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1">
-        <v>45915.22928240741</v>
+        <v>45931.22928240741</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Online Shopping</v>
+        <v>Movie</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
-        <v>45912.22928240741</v>
+        <v>45911.22928240741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>